<commit_message>
Intento de OLS pero da cosas raras
</commit_message>
<xml_diff>
--- a/GovernmentBondPrices_UnitedStates.xlsx
+++ b/GovernmentBondPrices_UnitedStates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fubeda/Library/CloudStorage/Dropbox/Clases/UPM/Renta Fija/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8228f603a68a6bd4/Escritorio/MÁSTER/Module 2/Computational Methods Applied to Finance/Entregas/Entrega 1/ComputationalMethodsMEFI/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C15CBC78-B029-6B4C-BF54-E0197DD403DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-75" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="3" r:id="rId1"/>
@@ -670,16 +670,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC395FB8-0503-F045-8A5F-4ACC88403B76}">
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="217" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection sqref="A1:J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -711,7 +711,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -743,7 +743,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -775,7 +775,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -807,7 +807,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -839,7 +839,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -871,7 +871,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -900,7 +900,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -932,7 +932,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -964,7 +964,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -996,7 +996,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -1025,7 +1025,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -1057,7 +1057,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -1089,7 +1089,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -1118,7 +1118,7 @@
         <v>45986</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -1150,7 +1150,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>21</v>
       </c>
@@ -1179,7 +1179,7 @@
         <v>45985</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>22</v>
       </c>
@@ -1211,7 +1211,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>23</v>
       </c>
@@ -1240,7 +1240,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>24</v>
       </c>
@@ -1273,7 +1273,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>25</v>
       </c>
@@ -1302,7 +1302,7 @@
         <v>45986</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>26</v>
       </c>
@@ -1334,7 +1334,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>27</v>
       </c>
@@ -1363,7 +1363,7 @@
         <v>45987</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>28</v>
       </c>
@@ -1395,7 +1395,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>29</v>
       </c>
@@ -1427,7 +1427,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>30</v>
       </c>
@@ -1460,7 +1460,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>31</v>
       </c>
@@ -1489,7 +1489,7 @@
         <v>45980</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>32</v>
       </c>
@@ -1521,7 +1521,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>33</v>
       </c>

</xml_diff>